<commit_message>
Fix are_points_matching function to manage depolarization points. About survey verification: print missed survey types that are not parsed by the tool but existing in the survey files. Modify survey result fule to display: DC_SYS name and Survey name separately, show DC_SYS sheet and Survey type. Add verification of platform OSP and of IATPM_Tags and IATPM_Version_Tags. Add some different survey type names. For switches verification, add possibility to create left and right points from the centre point when not existing in survey file. Add suffixes _G and _D in addition to _L and _R. Fix joint names generating mechanism to work with V4 (with no IVB). Start reworking the verification of platform.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_dc_tu_verification.xlsx
+++ b/prj/src/templates/template_dc_tu_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC4D9A4-ED94-4C2A-A971-F52C14818502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA6562D-EA9F-4FF5-8E9B-4A6923134312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Author</t>
   </si>
@@ -79,6 +79,12 @@
   <si>
     <t>Analysis of ADD_VERIF_XXX
 DC_TU Verification</t>
+  </si>
+  <si>
+    <t>DC_TU_Verification_Tool:</t>
+  </si>
+  <si>
+    <t>v1_0_1</t>
   </si>
 </sst>
 </file>
@@ -323,7 +329,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,30 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -363,33 +345,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -403,6 +358,61 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -899,7 +909,7 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A6:G29"/>
+  <dimension ref="A6:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:F20"/>
@@ -907,157 +917,165 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="11" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="11"/>
+    <col min="1" max="2" width="16.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="12"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="24"/>
-      <c r="C23" s="25" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="24"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="24"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="24"/>
+      <c r="D30" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1091,34 +1109,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="3"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:H2" xr:uid="{D8CA666F-C951-4E28-B85E-ED54F83BCF49}">
@@ -1182,26 +1200,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="3"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{9DE04395-FA11-44AD-A84B-74BB607C46AB}">

</xml_diff>

<commit_message>
Change Excel names from tol to tolerance. Update tool versions managing.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_dc_tu_verification.xlsx
+++ b/prj/src/templates/template_dc_tu_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA6562D-EA9F-4FF5-8E9B-4A6923134312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E446A335-61CE-4846-AEBD-9944CB624C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Author</t>
   </si>
@@ -81,10 +81,7 @@
 DC_TU Verification</t>
   </si>
   <si>
-    <t>DC_TU_Verification_Tool:</t>
-  </si>
-  <si>
-    <t>v1_0_1</t>
+    <t>DC_TU_Checking Version:</t>
   </si>
 </sst>
 </file>
@@ -360,60 +357,60 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -938,62 +935,62 @@
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
@@ -1063,19 +1060,17 @@
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="13"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1109,34 +1104,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="29" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:H2" xr:uid="{D8CA666F-C951-4E28-B85E-ED54F83BCF49}">
@@ -1200,26 +1195,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="29" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{9DE04395-FA11-44AD-A84B-74BB607C46AB}">

</xml_diff>

<commit_message>
Change version of DC_TU Verification to 1.1, so that it uses the new yes/no behavior, and adapt the template to be the same way as for survey.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_dc_tu_verification.xlsx
+++ b/prj/src/templates/template_dc_tu_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E446A335-61CE-4846-AEBD-9944CB624C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76833F16-FB3D-4761-BCC3-8F1688768DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="5" r:id="rId1"/>
@@ -531,23 +531,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>746984</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>154753</xdr:rowOff>
+      <xdr:colOff>1513915</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>188819</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="Hitachi_Hitachi_STS_orizz_Project_and_External_Documents_Orizzontale">
+        <xdr:cNvPr id="3" name="Image 2" descr="Hitachi_Hitachi_STS_orizz_Project_and_External_Documents_Orizzontale">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3A8CD73-423F-4319-86A9-F8B0E5D29D1A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C41A7CDE-A4D5-4037-BFDF-9979AB9500DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -570,8 +570,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="320040" y="367665"/>
-          <a:ext cx="4408394" cy="387163"/>
+          <a:off x="1086971" y="605118"/>
+          <a:ext cx="4416238" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -607,9 +607,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,7 +647,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -753,7 +753,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -895,7 +895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
Set the zoom level on template header file to 100% as for the other templates.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_dc_tu_verification.xlsx
+++ b/prj/src/templates/template_dc_tu_verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76833F16-FB3D-4761-BCC3-8F1688768DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C85943-9EED-4746-BB4F-7E56AD572B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
   </bookViews>
@@ -908,7 +908,7 @@
   </sheetPr>
   <dimension ref="A6:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>